<commit_message>
Fixed an issue with result tables not being saved properly
</commit_message>
<xml_diff>
--- a/Result Tables/Model.result.tables_2019.xlsx
+++ b/Result Tables/Model.result.tables_2019.xlsx
@@ -6,13 +6,18 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LDMC" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="nb.stem" sheetId="7" state="visible" r:id="rId1"/>
+    <sheet name="area.bunch" sheetId="8" state="visible" r:id="rId2"/>
+    <sheet name="prop.flower" sheetId="9" state="visible" r:id="rId3"/>
+    <sheet name="stem.height" sheetId="10" state="visible" r:id="rId4"/>
+    <sheet name="SLA" sheetId="11" state="visible" r:id="rId5"/>
+    <sheet name="LDMC" sheetId="12" state="visible" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -23,15 +28,30 @@
     <t xml:space="preserve">Std. Error</t>
   </si>
   <si>
+    <t xml:space="preserve">z value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pr(&gt;|z|)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Intercept)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">soil_water2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR</t>
+  </si>
+  <si>
     <t xml:space="preserve">t value</t>
   </si>
   <si>
     <t xml:space="preserve">Pr(&gt;|t|)</t>
   </si>
   <si>
-    <t xml:space="preserve">(Intercept)</t>
-  </si>
-  <si>
     <t xml:space="preserve">management22013</t>
   </si>
   <si>
@@ -39,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">management2Fichte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAR</t>
   </si>
 </sst>
 </file>
@@ -63,12 +80,17 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -102,10 +124,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,16 +444,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>156.986</v>
+        <v>1.455</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>8.082</v>
+        <v>0.476</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>19.425</v>
+        <v>3.054</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0</v>
+        <v>0.0023</v>
       </c>
     </row>
     <row r="3">
@@ -438,16 +461,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-2.881</v>
+        <v>-0.074</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>3.574</v>
+        <v>0.028</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-0.806</v>
+        <v>-2.621</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.4224</v>
+        <v>0.0088</v>
       </c>
     </row>
     <row r="4">
@@ -455,16 +478,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>-8.818</v>
+        <v>0.037</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>6.745</v>
+        <v>0.018</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>-1.307</v>
+        <v>2.024</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.1946</v>
+        <v>0.0429</v>
       </c>
     </row>
     <row r="5">
@@ -472,6 +495,535 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>5.471</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>-2.649</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>-8.787</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>-0.146</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.426</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>-0.342</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.7335</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>0.487</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.807</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.4217</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>1.717</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>3.654</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.0004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>-13.056</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>3.837</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>-3.403</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>4.556</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1.691</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>2.694</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.0085</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>2.899</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>3.201</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.3677</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>5.135</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>3.219</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>1.595</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.1143</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>0.424</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>3.741</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>60.699</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>-0.135</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>0.087</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>-1.546</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.1257</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-0.654</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>0.123</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-5.309</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>-0.748</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>-7.787</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>38.913</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>2.319</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>16.778</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1.022</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>0.557</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.5793</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-0.265</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>1.935</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-0.137</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.8916</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>4.725</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>1.946</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>2.429</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.0172</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>-0.271</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-4.058</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>156.986</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>8.082</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>19.425</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>-2.881</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>3.574</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>-0.806</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.4224</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-8.818</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>6.745</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-1.307</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.1946</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>-22.833</v>
       </c>
       <c r="C5" s="2" t="n">
@@ -486,7 +1038,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.521</v>

</xml_diff>